<commit_message>
Update batch import worksheet with better holotype instructions
</commit_message>
<xml_diff>
--- a/themes/morphosource/static/MorphoSourceBatchImportWorksheet.xlsx
+++ b/themes/morphosource/static/MorphoSourceBatchImportWorksheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmw110/rapidvm/html/themes/morphosource/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmw110/ms_prod/themes/morphosource/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3573B9D8-B6B4-3649-AB56-C5CD8A10EA4F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1DA088-C740-4943-ABAD-651D1452ADE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3700" yWindow="460" windowWidth="22280" windowHeight="15520" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -442,9 +442,6 @@
     <t>General description of specimen physical content</t>
   </si>
   <si>
-    <t>Holotype</t>
-  </si>
-  <si>
     <t>Sex of specimen</t>
   </si>
   <si>
@@ -776,6 +773,9 @@
   </si>
   <si>
     <t>Side of specimen depicted by media, if different from what was entered in the general information for the media. This is an optional drop-down field. To enter a value here, enter the exact text string from the MorphoSource drop-down (minus any quotes). Possible values for this field include: "Not Applicable", "Unknown", "Left", "Right", "Midline".</t>
+  </si>
+  <si>
+    <t>Holotype. This is an optional drop-down field. If nothing is entered here, the holotype status will be unset by default. To enter a value here, either enter the exact text string from the MorphoSource drop-down (minus any quotes) or the numeric code associated with the holotype status (minus any parentheses). Possible values for this field include: "Yes" (0), "No" (1). IMPORTANT: Please note here that the "Yes" value is paired with numeric value 0, and "No" is paired with numeric value 1, and NOT the reverse.</t>
   </si>
 </sst>
 </file>
@@ -1271,8 +1271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BT1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CB3" sqref="CB3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1891,331 +1891,331 @@
         <v>137</v>
       </c>
       <c r="L3" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="M3" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="N3" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="O3" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="P3" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="Q3" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="R3" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="S3" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="T3" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="T3" s="11" t="s">
+      <c r="U3" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="U3" s="11" t="s">
+      <c r="V3" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="V3" s="11" t="s">
+      <c r="W3" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="W3" s="11" t="s">
+      <c r="X3" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="X3" s="11" t="s">
+      <c r="Y3" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="Y3" s="11" t="s">
+      <c r="Z3" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="Z3" s="11" t="s">
+      <c r="AA3" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AA3" s="11" t="s">
+      <c r="AB3" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="AB3" s="11" t="s">
+      <c r="AC3" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="AC3" s="11" t="s">
+      <c r="AD3" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="AD3" s="11" t="s">
+      <c r="AE3" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="AE3" s="11" t="s">
+      <c r="AF3" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="AF3" s="11" t="s">
+      <c r="AG3" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="AG3" s="11" t="s">
+      <c r="AH3" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="AH3" s="11" t="s">
+      <c r="AI3" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="AI3" s="11" t="s">
+      <c r="AJ3" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="AJ3" s="11" t="s">
+      <c r="AK3" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AK3" s="11" t="s">
+      <c r="AL3" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AL3" s="11" t="s">
+      <c r="AM3" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="AM3" s="11" t="s">
+      <c r="AN3" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="AN3" s="11" t="s">
+      <c r="AO3" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="AO3" s="11" t="s">
+      <c r="AP3" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="AP3" s="11" t="s">
+      <c r="AQ3" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="AQ3" s="11" t="s">
+      <c r="AR3" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="AR3" s="11" t="s">
+      <c r="AS3" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="AS3" s="11" t="s">
+      <c r="AT3" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="AT3" s="11" t="s">
+      <c r="AU3" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="AU3" s="11" t="s">
+      <c r="AV3" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="AW3" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="AV3" s="11" t="s">
+      <c r="AX3" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="AY3" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="AZ3" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="BA3" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="BB3" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="BC3" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="BD3" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="BE3" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="BF3" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="AW3" s="11" t="s">
+      <c r="BG3" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="BH3" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="BI3" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="BJ3" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="BK3" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="BL3" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="BM3" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="BN3" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="BO3" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="BP3" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="BQ3" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="BR3" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="BS3" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="BT3" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="BU3" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="BV3" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="BW3" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="BX3" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="BY3" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="BZ3" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="CA3" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="CB3" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="CC3" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="CD3" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="CE3" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="AX3" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="AY3" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="AZ3" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="BA3" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="BB3" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="BC3" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="BD3" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="BE3" s="11" t="s">
+      <c r="CF3" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="CG3" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="CH3" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="CI3" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="CJ3" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="CK3" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="CL3" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="BF3" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="BG3" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="BH3" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="BI3" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="BJ3" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="BK3" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="BL3" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="BM3" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="BN3" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="BO3" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="BP3" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="BQ3" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="BR3" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="BS3" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="BT3" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="BU3" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="BV3" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="BW3" s="11" t="s">
+      <c r="CM3" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="CN3" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="CO3" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="CP3" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="BX3" s="11" t="s">
+      <c r="CQ3" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="BY3" s="11" t="s">
+      <c r="CR3" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="BZ3" s="11" t="s">
+      <c r="CS3" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="CA3" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="CB3" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="CC3" s="11" t="s">
+      <c r="CT3" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="CD3" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="CE3" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="CF3" s="11" t="s">
+      <c r="CU3" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="CV3" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="CG3" s="11" t="s">
+      <c r="CW3" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="CX3" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="CY3" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="CZ3" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="CH3" s="11" t="s">
+      <c r="DA3" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="CI3" s="11" t="s">
+      <c r="DB3" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="CJ3" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="CK3" s="11" t="s">
+      <c r="DC3" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="DD3" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="DE3" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="DF3" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="DG3" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="CL3" s="11" t="s">
+      <c r="DH3" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="DI3" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="DJ3" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="DK3" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="DL3" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="CM3" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="CN3" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="CO3" s="11" t="s">
+      <c r="DM3" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="DN3" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="CP3" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="CQ3" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="CR3" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="CS3" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="CT3" s="11" t="s">
+      <c r="DO3" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="DP3" s="11" t="s">
         <v>245</v>
-      </c>
-      <c r="CU3" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="CV3" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="CW3" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="CX3" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="CY3" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="CZ3" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="DA3" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="DB3" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="DC3" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="DD3" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="DE3" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="DF3" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="DG3" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="DH3" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="DI3" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="DJ3" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="DK3" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="DL3" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="DM3" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="DN3" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="DO3" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="DP3" s="11" t="s">
-        <v>246</v>
       </c>
       <c r="ALV3"/>
       <c r="ALW3"/>
@@ -2236,7 +2236,7 @@
     <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="AV4" s="12"/>
       <c r="BC4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -2266,136 +2266,136 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" t="s">
         <v>199</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>200</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>201</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>202</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>203</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>204</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>205</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>206</v>
-      </c>
-      <c r="I1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" t="s">
         <v>208</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>209</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>210</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>211</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>212</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>213</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>214</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>215</v>
-      </c>
-      <c r="I2" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E3" t="s">
         <v>217</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>218</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>219</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>220</v>
-      </c>
-      <c r="I3" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
+        <v>221</v>
+      </c>
+      <c r="F4" t="s">
         <v>222</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>223</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>224</v>
-      </c>
-      <c r="I4" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
+        <v>225</v>
+      </c>
+      <c r="F5" t="s">
         <v>226</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>227</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>228</v>
-      </c>
-      <c r="I5" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F6" t="s">
+        <v>229</v>
+      </c>
+      <c r="G6" t="s">
         <v>230</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>231</v>
-      </c>
-      <c r="I6" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>